<commit_message>
browser level directory support for extent reports
</commit_message>
<xml_diff>
--- a/dataxls/testcases.xlsx
+++ b/dataxls/testcases.xlsx
@@ -6,13 +6,12 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId4"/>
-    <sheet name="Sheet 2" sheetId="2" r:id="rId5"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="23">
   <si>
     <t>Table 1</t>
   </si>
@@ -81,9 +80,6 @@
   </si>
   <si>
     <t>Abercrombie &amp; Fitch</t>
-  </si>
-  <si>
-    <t>Karl Lagerfeld</t>
   </si>
 </sst>
 </file>
@@ -343,7 +339,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -405,12 +401,6 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1743,176 +1733,4 @@
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <pageSetUpPr fitToPage="1"/>
-  </sheetPr>
-  <dimension ref="A1:E11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col min="1" max="5" width="16.3516" style="21" customWidth="1"/>
-    <col min="6" max="16384" width="16.3516" style="21" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" ht="27.65" customHeight="1">
-      <c r="A1" t="s" s="2">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="4"/>
-    </row>
-    <row r="2" ht="20.25" customHeight="1">
-      <c r="A2" t="s" s="22">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s" s="22">
-        <v>2</v>
-      </c>
-      <c r="C2" t="s" s="22">
-        <v>3</v>
-      </c>
-      <c r="D2" t="s" s="22">
-        <v>4</v>
-      </c>
-      <c r="E2" t="s" s="22">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" ht="20.25" customHeight="1">
-      <c r="A3" t="s" s="17">
-        <v>12</v>
-      </c>
-      <c r="B3" t="s" s="18">
-        <v>23</v>
-      </c>
-      <c r="C3" t="s" s="19">
-        <v>14</v>
-      </c>
-      <c r="D3" s="11"/>
-      <c r="E3" t="s" s="19">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" ht="20.05" customHeight="1">
-      <c r="A4" t="s" s="7">
-        <v>12</v>
-      </c>
-      <c r="B4" t="s" s="8">
-        <v>13</v>
-      </c>
-      <c r="C4" t="s" s="9">
-        <v>14</v>
-      </c>
-      <c r="D4" s="12"/>
-      <c r="E4" t="s" s="9">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" ht="20.05" customHeight="1">
-      <c r="A5" t="s" s="7">
-        <v>15</v>
-      </c>
-      <c r="B5" s="13"/>
-      <c r="C5" t="s" s="9">
-        <v>16</v>
-      </c>
-      <c r="D5" s="12"/>
-      <c r="E5" t="s" s="9">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" ht="20.05" customHeight="1">
-      <c r="A6" t="s" s="7">
-        <v>15</v>
-      </c>
-      <c r="B6" s="13"/>
-      <c r="C6" t="s" s="9">
-        <v>8</v>
-      </c>
-      <c r="D6" s="12"/>
-      <c r="E6" t="s" s="9">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" ht="20.05" customHeight="1">
-      <c r="A7" t="s" s="7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s" s="8">
-        <v>19</v>
-      </c>
-      <c r="C7" t="s" s="9">
-        <v>20</v>
-      </c>
-      <c r="D7" t="s" s="9">
-        <v>21</v>
-      </c>
-      <c r="E7" t="s" s="9">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" ht="20.05" customHeight="1">
-      <c r="A8" t="s" s="14">
-        <v>6</v>
-      </c>
-      <c r="B8" t="s" s="15">
-        <v>9</v>
-      </c>
-      <c r="C8" t="s" s="16">
-        <v>8</v>
-      </c>
-      <c r="D8" t="s" s="16">
-        <v>10</v>
-      </c>
-      <c r="E8" t="s" s="16">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" ht="20.05" customHeight="1">
-      <c r="A9" t="s" s="17">
-        <v>6</v>
-      </c>
-      <c r="B9" t="s" s="18">
-        <v>22</v>
-      </c>
-      <c r="C9" t="s" s="19">
-        <v>8</v>
-      </c>
-      <c r="D9" s="11"/>
-      <c r="E9" t="s" s="19">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" ht="20.05" customHeight="1">
-      <c r="A10" s="20"/>
-      <c r="B10" s="13"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-    </row>
-    <row r="11" ht="20.05" customHeight="1">
-      <c r="A11" s="20"/>
-      <c r="B11" s="13"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:E1"/>
-  </mergeCells>
-  <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
-  <headerFooter>
-    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
 </file>
</xml_diff>